<commit_message>
changed csv files a little
</commit_message>
<xml_diff>
--- a/CsvFiles/StarCitizienShipWeaponDatabase.xlsx
+++ b/CsvFiles/StarCitizienShipWeaponDatabase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42de4e58389d54ac/Dokument/school/1DV503 Databasteknik/Database-Assignment-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42de4e58389d54ac/Dokument/school/1DV503 Databasteknik/Database-Mini-Project/CsvFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1527" documentId="8_{8AF52736-FF23-49A2-A830-9473FA8973EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC2934C0-91E9-431C-A64B-F6C29D52F6D5}"/>
+  <xr:revisionPtr revIDLastSave="1529" documentId="8_{8AF52736-FF23-49A2-A830-9473FA8973EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE5C369E-2137-4536-A806-A3FA72EBF797}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{670DD1E5-E9B3-493F-94E8-0619D74DCA8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{670DD1E5-E9B3-493F-94E8-0619D74DCA8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ships" sheetId="1" r:id="rId1"/>
@@ -804,60 +804,30 @@
     <t>HUR-L1</t>
   </si>
   <si>
-    <t>Green Glade Station</t>
-  </si>
-  <si>
-    <t>Beautiful Glen Station</t>
-  </si>
-  <si>
     <t>HUR-L2</t>
   </si>
   <si>
-    <t>Faithful Dream Station</t>
-  </si>
-  <si>
     <t>HUR-L3</t>
   </si>
   <si>
-    <t>Thundering Express Station</t>
-  </si>
-  <si>
     <t>HUR-L4</t>
   </si>
   <si>
-    <t>Melodic Fields Station</t>
-  </si>
-  <si>
     <t>HUR-L5</t>
   </si>
   <si>
-    <t>High Course Station</t>
-  </si>
-  <si>
     <t>CRU-L1</t>
   </si>
   <si>
-    <t>Ambitious Dream Station</t>
-  </si>
-  <si>
     <t>CRU-L4</t>
   </si>
   <si>
-    <t>Shallow Field Station</t>
-  </si>
-  <si>
     <t>ARC-L1</t>
   </si>
   <si>
-    <t>Wide Forest Station</t>
-  </si>
-  <si>
     <t>MIC-L1</t>
   </si>
   <si>
-    <t>Shallow Frontier Station</t>
-  </si>
-  <si>
     <t>Sentient</t>
   </si>
   <si>
@@ -1333,6 +1303,36 @@
   </si>
   <si>
     <t>Area18, Orison</t>
+  </si>
+  <si>
+    <t>Green Glade Station (HUR-L1)</t>
+  </si>
+  <si>
+    <t>Beautiful Glen Station (CRU-L5)</t>
+  </si>
+  <si>
+    <t>Faithful Dream Station (HUR-L2)</t>
+  </si>
+  <si>
+    <t>Thundering Express Station (HUR-L3)</t>
+  </si>
+  <si>
+    <t>Melodic Fields Station (HUR-L4)</t>
+  </si>
+  <si>
+    <t>High Course Station (HUR-L5)</t>
+  </si>
+  <si>
+    <t>Ambitious Dream Station (CRU-L1)</t>
+  </si>
+  <si>
+    <t>Shallow Field Station (CRU-L4)</t>
+  </si>
+  <si>
+    <t>Wide Forest Station (ARC-L1)</t>
+  </si>
+  <si>
+    <t>Shallow Frontier Station (MIC-L1)</t>
   </si>
 </sst>
 </file>
@@ -1804,7 +1804,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1833,13 +1833,13 @@
         <v>235</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>12</v>
@@ -1859,13 +1859,13 @@
         <v>235</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="F3" s="1">
         <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>12</v>
@@ -1882,16 +1882,16 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>12</v>
@@ -1917,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>12</v>
@@ -1963,7 +1963,7 @@
         <v>235</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="F7" s="1">
         <v>40</v>
@@ -2021,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>12</v>
@@ -2067,7 +2067,7 @@
         <v>235</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -2116,7 +2116,7 @@
         <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>40</v>
@@ -2142,7 +2142,7 @@
         <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>43</v>
@@ -2151,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>12</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>40</v>
@@ -2168,7 +2168,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>45</v>
@@ -2177,7 +2177,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>12</v>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>40</v>
@@ -2194,7 +2194,7 @@
         <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>33</v>
@@ -2203,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>12</v>
@@ -2220,16 +2220,16 @@
         <v>48</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>12</v>
@@ -2246,7 +2246,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>22</v>
@@ -2272,7 +2272,7 @@
         <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>38</v>
@@ -2298,7 +2298,7 @@
         <v>54</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>45</v>
@@ -2307,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>12</v>
@@ -2324,10 +2324,10 @@
         <v>56</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="F21" s="1">
         <v>30</v>
@@ -2350,7 +2350,7 @@
         <v>59</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>22</v>
@@ -2359,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>60</v>
@@ -2370,7 +2370,7 @@
         <v>62</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>63</v>
@@ -2385,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>12</v>
@@ -2411,7 +2411,7 @@
         <v>4</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>12</v>
@@ -2437,7 +2437,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>12</v>
@@ -2454,7 +2454,7 @@
         <v>71</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>22</v>
@@ -2463,7 +2463,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>12</v>
@@ -2480,7 +2480,7 @@
         <v>73</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>61</v>
@@ -2489,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>12</v>
@@ -2541,7 +2541,7 @@
         <v>576</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>12</v>
@@ -2561,7 +2561,7 @@
         <v>235</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="F30" s="1">
         <v>46</v>
@@ -2593,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>12</v>
@@ -2610,7 +2610,7 @@
         <v>86</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>22</v>
@@ -2619,7 +2619,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>12</v>
@@ -2636,7 +2636,7 @@
         <v>89</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>90</v>
@@ -2656,7 +2656,7 @@
         <v>91</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>92</v>
@@ -2682,7 +2682,7 @@
         <v>94</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>95</v>
@@ -2708,7 +2708,7 @@
         <v>97</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>98</v>
@@ -2734,7 +2734,7 @@
         <v>100</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>101</v>
@@ -2760,7 +2760,7 @@
         <v>103</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>104</v>
@@ -2769,7 +2769,7 @@
         <v>235</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="F38" s="2">
         <v>32</v>
@@ -2786,7 +2786,7 @@
         <v>105</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>106</v>
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>12</v>
@@ -2812,13 +2812,13 @@
         <v>107</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>108</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>33</v>
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>12</v>
@@ -2838,13 +2838,13 @@
         <v>109</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>110</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>61</v>
@@ -2853,7 +2853,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>12</v>
@@ -2864,7 +2864,7 @@
         <v>111</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>112</v>
@@ -2879,7 +2879,7 @@
         <v>6</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>12</v>
@@ -2890,7 +2890,7 @@
         <v>113</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>114</v>
@@ -2916,7 +2916,7 @@
         <v>116</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>117</v>
@@ -2942,7 +2942,7 @@
         <v>118</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>119</v>
@@ -2951,7 +2951,7 @@
         <v>151</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="F45" s="1">
         <v>8</v>
@@ -2968,13 +2968,13 @@
         <v>120</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>121</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>45</v>
@@ -2994,16 +2994,16 @@
         <v>122</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="F47" s="1">
         <v>4</v>
@@ -3017,16 +3017,16 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>124</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>61</v>
@@ -3043,10 +3043,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>125</v>
@@ -3055,7 +3055,7 @@
         <v>151</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
@@ -3069,16 +3069,16 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>126</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>61</v>
@@ -3087,7 +3087,7 @@
         <v>0</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>12</v>
@@ -3098,7 +3098,7 @@
         <v>127</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>128</v>
@@ -3124,7 +3124,7 @@
         <v>129</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>130</v>
@@ -3150,13 +3150,13 @@
         <v>131</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>22</v>
@@ -3176,7 +3176,7 @@
         <v>133</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>134</v>
@@ -3202,7 +3202,7 @@
         <v>135</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>136</v>
@@ -3228,16 +3228,16 @@
         <v>137</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>138</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="F56" s="2">
         <v>96</v>
@@ -3254,7 +3254,7 @@
         <v>139</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>140</v>
@@ -3280,16 +3280,16 @@
         <v>141</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>142</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="F58" s="2">
         <v>96</v>
@@ -3303,7 +3303,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>75</v>
@@ -3315,7 +3315,7 @@
         <v>235</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="F59" s="1">
         <v>12</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>75</v>
@@ -3341,7 +3341,7 @@
         <v>235</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="F60" s="2">
         <v>12</v>
@@ -3355,16 +3355,16 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="C61" s="1">
         <v>2781000</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>22</v>
@@ -3373,15 +3373,15 @@
         <v>0</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>40</v>
@@ -3390,7 +3390,7 @@
         <v>1492700</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>43</v>
@@ -3399,7 +3399,7 @@
         <v>0</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>12</v>
@@ -3407,10 +3407,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="C63" s="1">
         <v>5225300</v>
@@ -3419,7 +3419,7 @@
         <v>235</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="F63" s="1">
         <v>523</v>
@@ -3433,10 +3433,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C64" s="2">
         <v>1230000</v>
@@ -3445,7 +3445,7 @@
         <v>235</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="F64" s="2">
         <v>0</v>
@@ -3459,16 +3459,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C65" s="1">
         <v>654000</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>45</v>
@@ -3485,10 +3485,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C66" s="2">
         <v>791000</v>
@@ -3511,16 +3511,16 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C67" s="1">
         <v>839000</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>22</v>
@@ -3537,10 +3537,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C68" s="2">
         <v>9475100</v>
@@ -3549,13 +3549,13 @@
         <v>151</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="F68" s="2">
         <v>40</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>12</v>
@@ -3563,25 +3563,25 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C69" s="1">
         <v>9894000</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="F69" s="1">
         <v>12</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>12</v>
@@ -3589,19 +3589,19 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C70" s="1">
         <v>32294500</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="F70" s="1">
         <v>100</v>
@@ -3615,19 +3615,19 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="C71" s="2">
         <v>4925500</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="F71" s="2">
         <v>696</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>40</v>
@@ -3650,7 +3650,7 @@
         <v>406000</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>45</v>
@@ -3667,10 +3667,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C73" s="2">
         <v>3256400</v>
@@ -3693,10 +3693,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="C74" s="1">
         <v>4912500</v>
@@ -3719,10 +3719,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="C75" s="2">
         <v>5130500</v>
@@ -3731,7 +3731,7 @@
         <v>235</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="F75" s="2">
         <v>115</v>
@@ -3745,10 +3745,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="C76" s="1">
         <v>233000</v>
@@ -3757,13 +3757,13 @@
         <v>235</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="F76" s="1">
         <v>0</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>12</v>
@@ -3771,7 +3771,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>66</v>
@@ -3789,7 +3789,7 @@
         <v>24</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>12</v>
@@ -3797,7 +3797,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>85</v>
@@ -3806,10 +3806,10 @@
         <v>4248200</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="F78" s="1">
         <v>0</v>
@@ -3823,10 +3823,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C79" s="2">
         <v>780000</v>
@@ -3835,13 +3835,13 @@
         <v>235</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="F79" s="2">
         <v>0</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>12</v>
@@ -3849,10 +3849,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C80" s="1">
         <v>840000</v>
@@ -3861,13 +3861,13 @@
         <v>235</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="F80" s="1">
         <v>2</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>12</v>
@@ -3875,10 +3875,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C81" s="2">
         <v>870000</v>
@@ -3893,7 +3893,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>12</v>
@@ -3901,7 +3901,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>85</v>
@@ -3910,7 +3910,7 @@
         <v>1854500</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>11</v>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>85</v>
@@ -3936,7 +3936,7 @@
         <v>2259200</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>11</v>
@@ -3953,7 +3953,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>9</v>
@@ -3979,7 +3979,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>9</v>
@@ -4014,7 +4014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E321795-7F9A-4E3D-AE77-C356B404636E}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -4051,7 +4051,7 @@
         <v>146</v>
       </c>
       <c r="F1" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -5048,10 +5048,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B45" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -5063,7 +5063,7 @@
         <v>240</v>
       </c>
       <c r="F45" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G45">
         <v>5200</v>
@@ -5071,10 +5071,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B46" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -5086,7 +5086,7 @@
         <v>220</v>
       </c>
       <c r="F46" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="G46">
         <v>9550</v>
@@ -5094,10 +5094,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="B47" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C47">
         <v>3</v>
@@ -5109,7 +5109,7 @@
         <v>200</v>
       </c>
       <c r="F47" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="G47">
         <v>19200</v>
@@ -5117,10 +5117,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="B48" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -5140,10 +5140,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B49" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -5163,10 +5163,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="B50" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -5186,10 +5186,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="B51" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C51">
         <v>4</v>
@@ -5209,10 +5209,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="B52" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C52">
         <v>5</v>
@@ -5232,10 +5232,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B53" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C53">
         <v>6</v>
@@ -5255,10 +5255,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="B54" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -5270,7 +5270,7 @@
         <v>240</v>
       </c>
       <c r="F54" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="G54">
         <v>5300</v>
@@ -5278,10 +5278,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="B55" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C55">
         <v>2</v>
@@ -5293,7 +5293,7 @@
         <v>220</v>
       </c>
       <c r="F55" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="G55">
         <v>9950</v>
@@ -5301,10 +5301,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B56" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -5324,10 +5324,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B57" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C57">
         <v>4</v>
@@ -5339,7 +5339,7 @@
         <v>180</v>
       </c>
       <c r="F57" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="G57">
         <v>39050</v>
@@ -5347,10 +5347,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="B58" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C58">
         <v>5</v>
@@ -5362,7 +5362,7 @@
         <v>70</v>
       </c>
       <c r="F58" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="G58">
         <v>76700</v>
@@ -5370,10 +5370,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B59" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C59">
         <v>6</v>
@@ -5393,10 +5393,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="B60" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C60">
         <v>2</v>
@@ -5416,10 +5416,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="B61" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -5431,7 +5431,7 @@
         <v>240</v>
       </c>
       <c r="F61" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G61">
         <v>7450</v>
@@ -5439,10 +5439,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="B62" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C62">
         <v>2</v>
@@ -5454,7 +5454,7 @@
         <v>220</v>
       </c>
       <c r="F62" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="G62">
         <v>14150</v>
@@ -5462,10 +5462,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="B63" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -5477,7 +5477,7 @@
         <v>240</v>
       </c>
       <c r="F63" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="G63">
         <v>5200</v>
@@ -5485,10 +5485,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="B64" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C64">
         <v>3</v>
@@ -5500,7 +5500,7 @@
         <v>200</v>
       </c>
       <c r="F64" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="G64">
         <v>18650</v>
@@ -5508,10 +5508,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="B65" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C65">
         <v>2</v>
@@ -5523,7 +5523,7 @@
         <v>220</v>
       </c>
       <c r="F65" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="G65">
         <v>10600</v>
@@ -5531,10 +5531,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="B66" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C66">
         <v>4</v>
@@ -5546,7 +5546,7 @@
         <v>180</v>
       </c>
       <c r="F66" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="G66">
         <v>41950</v>
@@ -5554,10 +5554,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="B67" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C67">
         <v>5</v>
@@ -5569,7 +5569,7 @@
         <v>70</v>
       </c>
       <c r="F67" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="G67">
         <v>59300</v>
@@ -5577,10 +5577,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="B68" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C68">
         <v>6</v>
@@ -5592,7 +5592,7 @@
         <v>60</v>
       </c>
       <c r="F68" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="G68">
         <v>117150</v>
@@ -5600,10 +5600,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="B69" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C69">
         <v>3</v>
@@ -5615,7 +5615,7 @@
         <v>200</v>
       </c>
       <c r="F69" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="G69">
         <v>24250</v>
@@ -5623,10 +5623,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="B70" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -5646,10 +5646,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="B71" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C71">
         <v>2</v>
@@ -5669,10 +5669,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="B72" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C72">
         <v>3</v>
@@ -5692,10 +5692,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="B73" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C73">
         <v>4</v>
@@ -5715,10 +5715,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="B74" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C74">
         <v>5</v>
@@ -5738,10 +5738,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B75" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C75">
         <v>6</v>
@@ -5761,10 +5761,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>320</v>
+      </c>
+      <c r="B76" t="s">
         <v>330</v>
-      </c>
-      <c r="B76" t="s">
-        <v>340</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -5784,10 +5784,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="B77" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C77">
         <v>2</v>
@@ -5807,10 +5807,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="B78" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C78">
         <v>3</v>
@@ -5830,10 +5830,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="B79" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C79">
         <v>4</v>
@@ -5853,10 +5853,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="B80" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C80">
         <v>5</v>
@@ -5876,10 +5876,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="B81" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C81">
         <v>6</v>
@@ -5899,10 +5899,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="B82" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C82">
         <v>2</v>
@@ -5914,7 +5914,7 @@
         <v>600</v>
       </c>
       <c r="F82" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="G82">
         <v>6500</v>
@@ -5922,10 +5922,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="B83" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -5937,7 +5937,7 @@
         <v>720</v>
       </c>
       <c r="F83" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="G83">
         <v>4400</v>
@@ -5945,10 +5945,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="B84" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C84">
         <v>2</v>
@@ -5960,7 +5960,7 @@
         <v>600</v>
       </c>
       <c r="F84" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="G84">
         <v>7650</v>
@@ -5968,10 +5968,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="B85" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C85">
         <v>3</v>
@@ -5983,7 +5983,7 @@
         <v>500</v>
       </c>
       <c r="F85" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="G85">
         <v>13950</v>
@@ -5991,10 +5991,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="B86" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -6014,10 +6014,10 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="B87" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="C87">
         <v>2</v>
@@ -6037,10 +6037,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="B88" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="C88">
         <v>3</v>
@@ -6060,10 +6060,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="B89" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="C89">
         <v>3</v>
@@ -6075,7 +6075,7 @@
         <v>70</v>
       </c>
       <c r="F89" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="G89">
         <v>12900</v>
@@ -6234,8 +6234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4007CE-06A1-4D90-A56A-F9BBC31A4C0A}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6244,7 +6244,7 @@
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6444,7 +6444,7 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>251</v>
+        <v>418</v>
       </c>
       <c r="I7" t="s">
         <v>229</v>
@@ -6473,7 +6473,7 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>252</v>
+        <v>419</v>
       </c>
       <c r="I8" t="s">
         <v>229</v>
@@ -6481,7 +6481,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B9" t="s">
         <v>249</v>
@@ -6502,7 +6502,7 @@
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>254</v>
+        <v>420</v>
       </c>
       <c r="I9" t="s">
         <v>229</v>
@@ -6510,7 +6510,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B10" t="s">
         <v>249</v>
@@ -6531,7 +6531,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>256</v>
+        <v>421</v>
       </c>
       <c r="I10" t="s">
         <v>229</v>
@@ -6539,7 +6539,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B11" t="s">
         <v>249</v>
@@ -6560,7 +6560,7 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>258</v>
+        <v>422</v>
       </c>
       <c r="I11" t="s">
         <v>229</v>
@@ -6568,7 +6568,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B12" t="s">
         <v>249</v>
@@ -6589,7 +6589,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>260</v>
+        <v>423</v>
       </c>
       <c r="I12" t="s">
         <v>229</v>
@@ -6597,7 +6597,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B13" t="s">
         <v>249</v>
@@ -6618,7 +6618,7 @@
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>262</v>
+        <v>424</v>
       </c>
       <c r="I13" t="s">
         <v>229</v>
@@ -6626,7 +6626,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B14" t="s">
         <v>249</v>
@@ -6647,7 +6647,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>264</v>
+        <v>425</v>
       </c>
       <c r="I14" t="s">
         <v>229</v>
@@ -6655,7 +6655,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B15" t="s">
         <v>249</v>
@@ -6676,7 +6676,7 @@
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>266</v>
+        <v>426</v>
       </c>
       <c r="I15" t="s">
         <v>229</v>
@@ -6684,7 +6684,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B16" t="s">
         <v>249</v>
@@ -6705,7 +6705,7 @@
         <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>268</v>
+        <v>427</v>
       </c>
       <c r="I16" t="s">
         <v>229</v>
@@ -6735,27 +6735,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C1" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D1" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="D2" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6766,10 +6766,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D3" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -6780,52 +6780,52 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="D4" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="D5" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="D6" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D7" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>